<commit_message>
Laboju home lapu (profile.php)
kaut kas bija sačakarēts ar gui dēļ tās style kopā likšanas
</commit_message>
<xml_diff>
--- a/Dok/Kludu_zinojumu_arhivs.xlsx
+++ b/Dok/Kludu_zinojumu_arhivs.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krists\Documents\GitHub\MCVS\MCVS\Dok\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,8 +13,8 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
   <si>
     <t>Nr.</t>
   </si>
@@ -111,16 +106,6 @@
 4. Veicot pievienošanu jāuztaisa IF nosacījums - ja nav veiksmīgi pievienots - parādās kļūdas ziņojums, ja ir, parādās informatīvs ziņojums pēc kura lapa  pāriet uz main.php</t>
   </si>
   <si>
-    <t>Šis ir tikai informatīvs teksts - to vari izdzēst, kad esi iepazinies.
-Kad paņem kādu risināmo uzdevumu:
-1. Nomaini statusu uz P;
-2. Pieliec labojuma veicēju;
-Ja paspēj izlabot tikai, piemēram, 1. no abiem uzdevumiem - atstāj statusu P un komentāros pieraksti - izlabots 1. punkts.
-Ja ir izlaboti visi uzdevumi:
-1. Nomaini statusu uz A un iekrāso uzdevumu zaļā krāsā
-Ja kādi jautājumi - esmu Tavā rīcībā!</t>
-  </si>
-  <si>
     <t>1. Ievades lauka nosaukums un pats ievades lauks vienā rindā;
 2. Ievades laukus vajadzētu līdzināt pēc vienas vertikālas līnijas;
 3. Lietotāja lomas sarakstu vajag vienādā lielumā ar ievades laukiem;
@@ -132,8 +117,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -268,7 +253,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,7 +288,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -480,21 +465,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="1"/>
     <col min="2" max="2" width="10.42578125" customWidth="1"/>
@@ -505,7 +490,7 @@
     <col min="7" max="7" width="38.42578125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -528,7 +513,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -544,11 +529,9 @@
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="150">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -566,7 +549,7 @@
       </c>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -584,7 +567,7 @@
       </c>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="210">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -595,14 +578,14 @@
         <v>18</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="135">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -620,7 +603,7 @@
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="135">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -638,7 +621,7 @@
       </c>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -650,7 +633,7 @@
       <c r="E8" s="1"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -662,7 +645,7 @@
       <c r="E9" s="1"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -674,7 +657,7 @@
       <c r="E10" s="1"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -686,52 +669,52 @@
       <c r="E11" s="1"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12" s="1"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13" s="1"/>
       <c r="D13" s="5"/>
       <c r="E13" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14" s="1"/>
       <c r="D14" s="5"/>
       <c r="E14" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="A15" s="1"/>
       <c r="D15" s="5"/>
       <c r="E15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="A16" s="1"/>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4">
       <c r="A17" s="1"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="1"/>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4">
       <c r="A19" s="1"/>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4">
       <c r="A20" s="1"/>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="1"/>
       <c r="D21" s="5"/>
     </row>

</xml_diff>

<commit_message>
groupPlanning pogas tests V3 + atjaunots excel kļūdu dok.
</commit_message>
<xml_diff>
--- a/Dok/Kludu_zinojumu_arhivs.xlsx
+++ b/Dok/Kludu_zinojumu_arhivs.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krists\Documents\GitHub\MCVS\MCVS\Dok\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -13,8 +18,8 @@
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -22,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
   <si>
     <t>Nr.</t>
   </si>
@@ -36,9 +41,6 @@
     <t>Apraksts</t>
   </si>
   <si>
-    <t>Statuss</t>
-  </si>
-  <si>
     <t>A - atrisināts</t>
   </si>
   <si>
@@ -54,9 +56,6 @@
     <t>P - procesā</t>
   </si>
   <si>
-    <t>05.11.</t>
-  </si>
-  <si>
     <t>user-page.php</t>
   </si>
   <si>
@@ -69,8 +68,27 @@
     <t>profile.php</t>
   </si>
   <si>
+    <t>newUser.php</t>
+  </si>
+  <si>
+    <t>newCourse.php</t>
+  </si>
+  <si>
+    <t>newRoom.php</t>
+  </si>
+  <si>
     <t>1. Ievades lauka nosaukums un pats ievades lauks vienā rindā;
-2. Ievades lauka un pogas nosaukumi - latviski</t>
+2. Ievades laukus un checkbox izvēlnes vajadzētu līdzināt pēc vienas vertikālas līnijas;
+3. Pogu Pievienot vēlams centrēt;
+4. Veicot pievienošanu jāuztaisa IF nosacījums - ja nav veiksmīgi pievienots - parādās kļūdas ziņojums, ja ir, parādās informatīvs ziņojums pēc kura lapa  pāriet uz main.php</t>
+  </si>
+  <si>
+    <t>1. Jāpārskata pievienošanas forma sistēmā - DB ir jauni lauki un tie atšķiras no IS laukiem;
+2. Pēc pogas "Pievienot" ieraksts DB netiek pievienots.</t>
+  </si>
+  <si>
+    <t>1. Ievades lauka nosaukums un pats ievades lauks vienā rindā;
+2. Ievades lauka un pogas nosaukumi - latviski.</t>
   </si>
   <si>
     <t>1. Pārsaukt lapu par main.php;
@@ -78,47 +96,44 @@
 3. Meklēšanā - students un pasniedzējs pārvērst par vienu izvēlni - lietotājs;
 4. Pārskatīt visā lapā mīkstinājuma zīmes (pogām, lauku nosaukumiem);
 5. Pielikt home pogu (ko Kļaviņš gribēja);
-6. Meklēšanas izkārtojums - meklēšanas ievades laukus vajadzētu līdzināt pēc vienas vertikālas līnijas</t>
+6. Meklēšanas izkārtojums - meklēšanas ievades laukus vajadzētu līdzināt pēc vienas vertikālas līnijas.</t>
   </si>
   <si>
     <t>1. Sataisīt mīkstinājuma zīmes;
-2. Noņemt nost "TU ESI ADMIN..." :D</t>
-  </si>
-  <si>
-    <t>newUser.php</t>
-  </si>
-  <si>
-    <t>newCourse.php</t>
-  </si>
-  <si>
-    <t>newRoom.php</t>
-  </si>
-  <si>
-    <t>1. Ievades lauka nosaukums un pats ievades lauks vienā rindā;
-2. Ievades laukus vajadzētu līdzināt pēc vienas vertikālas līnijas;
-3. Pogu Pievienot vēlams centrēt
-4. Veicot pievienošanu jāuztaisa IF nosacījums - ja nav veiksmīgi pievienots - parādās kļūdas ziņojums, ja ir, parādās informatīvs ziņojums pēc kura lapa  pāriet uz main.php</t>
-  </si>
-  <si>
-    <t>1. Ievades lauka nosaukums un pats ievades lauks vienā rindā;
-2. Ievades laukus un checkbox izvēlnes vajadzētu līdzināt pēc vienas vertikālas līnijas;
-3. Pogu Pievienot vēlams centrēt
-4. Veicot pievienošanu jāuztaisa IF nosacījums - ja nav veiksmīgi pievienots - parādās kļūdas ziņojums, ja ir, parādās informatīvs ziņojums pēc kura lapa  pāriet uz main.php</t>
+2. Noņemt nost uzrakstu "TU ESI ADMINISTRATORS".</t>
   </si>
   <si>
     <t>1. Ievades lauka nosaukums un pats ievades lauks vienā rindā;
 2. Ievades laukus vajadzētu līdzināt pēc vienas vertikālas līnijas;
 3. Lietotāja lomas sarakstu vajag vienādā lielumā ar ievades laukiem;
-4. Pogu Pievienot vēlams centrēt
+4. Pogu Pievienot vēlams centrēt;
 5. Veicot pievienošanu jāuztaisa IF nosacījums - ja nav veiksmīgi pievienots - parādās kļūdas ziņojums, ja ir, parādās informatīvs ziņojums pēc kura lapa  pāriet uz main.php;
-6. Pareizrakstības kļūda: Perosnas kods --&gt; Personas kods (pārskati visas lapas, varbūt kko neesmu ieraudzījis)</t>
+6. Pareizrakstības kļūda: Perosnas kods --&gt; Personas kods (pārskati visas lapas, varbūt kko neesmu ieraudzījis).</t>
+  </si>
+  <si>
+    <t>1. Ievades lauka nosaukums un pats ievades lauks vienā rindā;
+2. Ievades laukus vajadzētu līdzināt pēc vienas vertikālas līnijas;
+3. Pogu Pievienot vēlams centrēt;
+4. Veicot pievienošanu jāuztaisa IF nosacījums - ja nav veiksmīgi pievienots - parādās kļūdas ziņojums, ja ir, parādās informatīvs ziņojums pēc kura lapa  pāriet uz main.php.</t>
+  </si>
+  <si>
+    <t>05.11.2015.</t>
+  </si>
+  <si>
+    <t>11.11.2015.</t>
+  </si>
+  <si>
+    <t>*Statusi:</t>
+  </si>
+  <si>
+    <t>Statuss*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -127,13 +142,34 @@
       <charset val="186"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -148,23 +184,37 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,258 +515,271 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="46.28515625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="38.42578125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="38.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="7"/>
+    </row>
+    <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="8"/>
+      <c r="G3" s="9"/>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" ht="210" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="45">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="F5" s="8"/>
+      <c r="G5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="8"/>
+      <c r="G7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="8"/>
+      <c r="G8" s="9"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="9"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="9"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="150">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" ht="30">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" ht="210">
-      <c r="A5" s="1">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="135">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" ht="135">
-      <c r="A7" s="1">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G7" s="5"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" s="1">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="1"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" s="1">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="1"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="1"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="1"/>
-      <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1"/>
-      <c r="D13" s="5"/>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="1"/>
-      <c r="D14" s="5"/>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="1"/>
-      <c r="D15" s="5"/>
-      <c r="E15" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="1"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="D21" s="5"/>
+      <c r="D21" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Papildināta DB un kļūdu ziņojumu excelis
</commit_message>
<xml_diff>
--- a/Dok/Kludu_zinojumu_arhivs.xlsx
+++ b/Dok/Kludu_zinojumu_arhivs.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Nr.</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>Statuss*</t>
+  </si>
+  <si>
+    <t>16.11.2015.</t>
+  </si>
+  <si>
+    <t>Pēc autorizācijas vajag atvērt atbilstošo lapu katrai lomai.</t>
   </si>
 </sst>
 </file>
@@ -526,7 +532,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -696,14 +702,22 @@
       <c r="F8" s="8"/>
       <c r="G8" s="9"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>8</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="6"/>
+      <c r="B9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="F9" s="8"/>
       <c r="G9" s="9"/>
     </row>

</xml_diff>

<commit_message>
Sākti Excel labojumi - index.php
</commit_message>
<xml_diff>
--- a/Dok/Kludu_zinojumu_arhivs.xlsx
+++ b/Dok/Kludu_zinojumu_arhivs.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Nr.</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Pēc autorizācijas vajag atvērt atbilstošo lapu katrai lomai.</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Krists</t>
   </si>
 </sst>
 </file>
@@ -531,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,9 +589,11 @@
         <v>18</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="8"/>
+        <v>29</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
@@ -604,7 +612,7 @@
       <c r="E3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="6"/>
       <c r="G3" s="9"/>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -623,7 +631,7 @@
       <c r="E4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="9"/>
     </row>
     <row r="5" spans="1:7" ht="210" x14ac:dyDescent="0.25">
@@ -642,7 +650,7 @@
       <c r="E5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="9"/>
     </row>
     <row r="6" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -661,7 +669,7 @@
       <c r="E6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="9"/>
     </row>
     <row r="7" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -680,7 +688,7 @@
       <c r="E7" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
@@ -699,7 +707,7 @@
       <c r="E8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -718,7 +726,7 @@
       <c r="E9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="9"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -729,7 +737,7 @@
       <c r="C10" s="6"/>
       <c r="D10" s="7"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="8"/>
+      <c r="F10" s="6"/>
       <c r="G10" s="9"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -740,7 +748,7 @@
       <c r="C11" s="6"/>
       <c r="D11" s="7"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="8"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="9"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Labojumi profile.php lapā > tagad main.php
</commit_message>
<xml_diff>
--- a/Dok/Kludu_zinojumu_arhivs.xlsx
+++ b/Dok/Kludu_zinojumu_arhivs.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
   <si>
     <t>Nr.</t>
   </si>
@@ -135,10 +135,10 @@
     <t>Pēc autorizācijas vajag atvērt atbilstošo lapu katrai lomai.</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>Krists</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -164,7 +164,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -183,6 +183,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -196,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -227,6 +239,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,7 +561,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -576,44 +599,46 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+      <c r="A2" s="14">
         <v>1</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" s="14">
+        <v>2</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="9"/>
+      <c r="F3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
@@ -772,14 +797,14 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="8" t="s">
+      <c r="E15" s="13" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="12" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Labojumi newUser.php lapā V1
</commit_message>
<xml_diff>
--- a/Dok/Kludu_zinojumu_arhivs.xlsx
+++ b/Dok/Kludu_zinojumu_arhivs.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
   <si>
     <t>Nr.</t>
   </si>
@@ -105,40 +105,68 @@
   <si>
     <t>1. Ievades lauka nosaukums un pats ievades lauks vienā rindā;
 2. Ievades laukus vajadzētu līdzināt pēc vienas vertikālas līnijas;
+3. Pogu Pievienot vēlams centrēt;
+4. Veicot pievienošanu jāuztaisa IF nosacījums - ja nav veiksmīgi pievienots - parādās kļūdas ziņojums, ja ir, parādās informatīvs ziņojums pēc kura lapa  pāriet uz main.php.</t>
+  </si>
+  <si>
+    <t>05.11.2015.</t>
+  </si>
+  <si>
+    <t>11.11.2015.</t>
+  </si>
+  <si>
+    <t>*Statusi:</t>
+  </si>
+  <si>
+    <t>Statuss*</t>
+  </si>
+  <si>
+    <t>16.11.2015.</t>
+  </si>
+  <si>
+    <t>Pēc autorizācijas vajag atvērt atbilstošo lapu katrai lomai.</t>
+  </si>
+  <si>
+    <t>Krists</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>19.11.2015.</t>
+  </si>
+  <si>
+    <t>header.php
+footer.php</t>
+  </si>
+  <si>
+    <t>1. Uzlikt tumši zilu vai violetu fonu</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>Mīkstinājuma zīmes vēl nav sataisītas…</t>
+  </si>
+  <si>
+    <t>main.php</t>
+  </si>
+  <si>
+    <t>1. Meklēšanas rezultātus attēlot tāpat kā groupPlanning.php lapā</t>
+  </si>
+  <si>
+    <t>Piemēram - ja nav atrasti rezultāti, izvadīt vienādu ziņojumu tabulas vidū, nevis augšā, utt.</t>
+  </si>
+  <si>
+    <t>1. Ievades lauka nosaukums un pats ievades lauks vienā rindā;
+2. Ievades laukus vajadzētu līdzināt pēc vienas vertikālas līnijas;
 3. Lietotāja lomas sarakstu vajag vienādā lielumā ar ievades laukiem;
 4. Pogu Pievienot vēlams centrēt;
 5. Veicot pievienošanu jāuztaisa IF nosacījums - ja nav veiksmīgi pievienots - parādās kļūdas ziņojums, ja ir, parādās informatīvs ziņojums pēc kura lapa  pāriet uz main.php;
-6. Pareizrakstības kļūda: Perosnas kods --&gt; Personas kods (pārskati visas lapas, varbūt kko neesmu ieraudzījis).</t>
-  </si>
-  <si>
-    <t>1. Ievades lauka nosaukums un pats ievades lauks vienā rindā;
-2. Ievades laukus vajadzētu līdzināt pēc vienas vertikālas līnijas;
-3. Pogu Pievienot vēlams centrēt;
-4. Veicot pievienošanu jāuztaisa IF nosacījums - ja nav veiksmīgi pievienots - parādās kļūdas ziņojums, ja ir, parādās informatīvs ziņojums pēc kura lapa  pāriet uz main.php.</t>
-  </si>
-  <si>
-    <t>05.11.2015.</t>
-  </si>
-  <si>
-    <t>11.11.2015.</t>
-  </si>
-  <si>
-    <t>*Statusi:</t>
-  </si>
-  <si>
-    <t>Statuss*</t>
-  </si>
-  <si>
-    <t>16.11.2015.</t>
-  </si>
-  <si>
-    <t>Pēc autorizācijas vajag atvērt atbilstošo lapu katrai lomai.</t>
-  </si>
-  <si>
-    <t>Krists</t>
-  </si>
-  <si>
-    <t>A</t>
+6. Pareizrakstības kļūda: Perosnas kods --&gt; Personas kods.</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -196,7 +224,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -204,11 +232,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -219,36 +276,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -558,10 +624,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,263 +638,347 @@
     <col min="4" max="4" width="46.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
-    <col min="7" max="7" width="38.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="38.42578125" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="10"/>
+    </row>
+    <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="12">
+        <v>3</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="195" x14ac:dyDescent="0.25">
+      <c r="A5" s="12">
+        <v>4</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="12"/>
+    </row>
+    <row r="6" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
+        <v>5</v>
+      </c>
+      <c r="B6" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="15"/>
+    </row>
+    <row r="7" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
+        <v>6</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+    </row>
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
+        <v>7</v>
+      </c>
+      <c r="B8" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="15">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="C9" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+    </row>
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="14">
-        <v>1</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="14" t="s">
+      <c r="B11" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="15">
         <v>11</v>
       </c>
-      <c r="D2" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A3" s="14">
-        <v>2</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="14" t="s">
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
         <v>12</v>
       </c>
-      <c r="D3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="G3" s="16"/>
-    </row>
-    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
-        <v>3</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="1:7" ht="210" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="6" t="s">
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
         <v>13</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="B14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
         <v>14</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="9"/>
-    </row>
-    <row r="7" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
-        <v>6</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="18">
         <v>15</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="9"/>
-    </row>
-    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
-        <v>7</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
-        <v>8</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="9"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6">
-        <v>9</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="9"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6">
-        <v>10</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="9"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="D17" s="3"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="D18" s="3"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="D19" s="3"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="D20" s="3"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="D21" s="3"/>
+      <c r="E21" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="D26" s="3"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F11:G11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Pēdējās izmaiņas, labots excel fails
</commit_message>
<xml_diff>
--- a/Dok/Kludu_zinojumu_arhivs.xlsx
+++ b/Dok/Kludu_zinojumu_arhivs.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>Nr.</t>
   </si>
@@ -146,9 +146,6 @@
     <t>P</t>
   </si>
   <si>
-    <t>Mīkstinājuma zīmes vēl nav sataisītas…</t>
-  </si>
-  <si>
     <t>main.php</t>
   </si>
   <si>
@@ -166,7 +163,19 @@
 6. Pareizrakstības kļūda: Perosnas kods --&gt; Personas kods.</t>
   </si>
   <si>
-    <t>s</t>
+    <t>5. punkts vēl nav pabeigts, pārējais ir ok (stilu newCourse un newRoom var stilot līdzīgi kā šo lapu)</t>
+  </si>
+  <si>
+    <t>20.11.2015.</t>
+  </si>
+  <si>
+    <t>header.php</t>
+  </si>
+  <si>
+    <t>1. Vajag uztaisīt uz ātro logo un ielikt favikonu</t>
+  </si>
+  <si>
+    <t>1. punkts vēl nav pabeigts - pabeigt ASAP!</t>
   </si>
 </sst>
 </file>
@@ -307,14 +316,14 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -626,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -726,7 +735,7 @@
         <v>28</v>
       </c>
       <c r="G4" s="12" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="195" x14ac:dyDescent="0.25">
@@ -740,7 +749,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>33</v>
@@ -748,7 +757,9 @@
       <c r="F5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5" s="12" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
@@ -766,9 +777,7 @@
       <c r="E6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="15" t="s">
-        <v>39</v>
-      </c>
+      <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
     <row r="7" spans="1:7" ht="135" x14ac:dyDescent="0.25">
@@ -855,27 +864,35 @@
         <v>30</v>
       </c>
       <c r="C11" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="16" t="s">
         <v>35</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>36</v>
       </c>
       <c r="E11" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="17"/>
+      <c r="F11" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
         <v>11</v>
       </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="16"/>
-      <c r="E12" s="15"/>
+      <c r="B12" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>6</v>
+      </c>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
     </row>
@@ -913,15 +930,15 @@
       <c r="G15" s="15"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="18">
+      <c r="A16" s="17">
         <v>15</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="18"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>

</xml_diff>

<commit_message>
Mazi labojumi visas malās
</commit_message>
<xml_diff>
--- a/Dok/Kludu_zinojumu_arhivs.xlsx
+++ b/Dok/Kludu_zinojumu_arhivs.xlsx
@@ -626,7 +626,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -636,8 +636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -809,25 +809,25 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="60">
-      <c r="A8" s="12">
+      <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="12" t="s">
+      <c r="E8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G8" s="12"/>
+      <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" ht="30">
       <c r="A9" s="15">

</xml_diff>

<commit_message>
Atkal visādi mazie labojumiņi
</commit_message>
<xml_diff>
--- a/Dok/Kludu_zinojumu_arhivs.xlsx
+++ b/Dok/Kludu_zinojumu_arhivs.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="44">
   <si>
     <t>Nr.</t>
   </si>
@@ -94,10 +94,6 @@
 6. Meklēšanas izkārtojums - meklēšanas ievades laukus vajadzētu līdzināt pēc vienas vertikālas līnijas.</t>
   </si>
   <si>
-    <t>1. Sataisīt mīkstinājuma zīmes;
-2. Noņemt nost uzrakstu "TU ESI ADMINISTRATORS".</t>
-  </si>
-  <si>
     <t>1. Ievades lauka nosaukums un pats ievades lauks vienā rindā;
 2. Ievades laukus vajadzētu līdzināt pēc vienas vertikālas līnijas;
 3. Pogu Pievienot vēlams centrēt;
@@ -136,9 +132,6 @@
   </si>
   <si>
     <t>1. Uzlikt tumši zilu vai violetu fonu</t>
-  </si>
-  <si>
-    <t>P</t>
   </si>
   <si>
     <t>main.php</t>
@@ -155,9 +148,6 @@
 6. Pareizrakstības kļūda: Perosnas kods --&gt; Personas kods.</t>
   </si>
   <si>
-    <t>5. punkts vēl nav pabeigts, pārējais ir ok (stilu newCourse un newRoom var stilot līdzīgi kā šo lapu)</t>
-  </si>
-  <si>
     <t>20.11.2015.</t>
   </si>
   <si>
@@ -167,16 +157,22 @@
     <t>1. Vajag uztaisīt uz ātro logo un ielikt favikonu</t>
   </si>
   <si>
-    <t>1. punkts vēl nav pabeigts - pabeigt ASAP!</t>
-  </si>
-  <si>
     <t>Arnis</t>
   </si>
   <si>
     <t xml:space="preserve">Pieliku vēl HOME pogu </t>
   </si>
   <si>
-    <t>4. punkts vel japabeidz</t>
+    <t>Krists, Arnis</t>
+  </si>
+  <si>
+    <t>VISA SISTĒMA</t>
+  </si>
+  <si>
+    <t>1.Sataisīt mīkstinājumzīmes</t>
+  </si>
+  <si>
+    <t>1. Noņemt nost uzrakstu "TU ESI ADMINISTRATORS".</t>
   </si>
 </sst>
 </file>
@@ -275,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -302,15 +298,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -325,6 +312,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -626,7 +619,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -636,8 +629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -665,7 +658,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>5</v>
@@ -679,7 +672,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="10" t="s">
         <v>11</v>
@@ -688,10 +681,10 @@
         <v>18</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G2" s="10"/>
     </row>
@@ -700,7 +693,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>12</v>
@@ -709,111 +702,103 @@
         <v>19</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G3" s="10"/>
+    </row>
+    <row r="4" spans="1:7" ht="30">
+      <c r="A4" s="10">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G3" s="10"/>
-    </row>
-    <row r="4" spans="1:7" ht="45">
-      <c r="A4" s="12">
-        <v>3</v>
-      </c>
-      <c r="B4" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="13" t="s">
+      <c r="F4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="10"/>
+    </row>
+    <row r="5" spans="1:7" ht="195">
+      <c r="A5" s="10">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5" s="10"/>
+    </row>
+    <row r="6" spans="1:7" ht="135">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="12" t="s">
+      <c r="E6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="195">
-      <c r="A5" s="12">
-        <v>4</v>
-      </c>
-      <c r="B5" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="12" t="s">
+      <c r="F6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:7" ht="135">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="G5" s="12" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="135">
-      <c r="A6" s="12">
-        <v>5</v>
-      </c>
-      <c r="B6" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="135">
-      <c r="A7" s="12">
-        <v>6</v>
-      </c>
-      <c r="B7" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>44</v>
-      </c>
+      <c r="F7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:7" ht="60">
       <c r="A8" s="10">
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>15</v>
@@ -822,53 +807,53 @@
         <v>17</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G8" s="10"/>
     </row>
     <row r="9" spans="1:7" ht="30">
-      <c r="A9" s="15">
+      <c r="A9" s="12">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
     </row>
     <row r="10" spans="1:7" ht="30">
       <c r="A10" s="10">
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="11" t="s">
-        <v>32</v>
-      </c>
       <c r="E10" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30">
@@ -876,86 +861,92 @@
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="19"/>
+        <v>38</v>
+      </c>
+      <c r="G11" s="16"/>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="10">
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10"/>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="12">
+        <v>12</v>
+      </c>
+      <c r="B13" s="18">
+        <v>42333</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="G12" s="10"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="15">
-        <v>12</v>
-      </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="15">
+      <c r="A14" s="12">
         <v>13</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="13"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="15">
+      <c r="A15" s="12">
         <v>14</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
     </row>
     <row r="16" spans="1:7">
-      <c r="A16" s="17">
+      <c r="A16" s="14">
         <v>15</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="14"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="14"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="1"/>
@@ -965,7 +956,7 @@
       <c r="A18" s="1"/>
       <c r="D18" s="3"/>
       <c r="E18" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:5">

</xml_diff>